<commit_message>
16th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">16/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">17/03/2020</t>
@@ -746,7 +749,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>832</v>
+        <v>882</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +765,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>20</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35">
@@ -770,7 +773,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36">
@@ -778,7 +781,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37">
@@ -786,7 +789,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
@@ -794,7 +797,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39">
@@ -802,7 +805,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40">
@@ -810,7 +813,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41">
@@ -818,7 +821,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42">
@@ -826,7 +829,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
@@ -834,7 +837,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44">
@@ -842,7 +845,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>153</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
@@ -850,7 +853,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46">
@@ -858,7 +861,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47">
@@ -866,7 +869,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48">
@@ -874,7 +877,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -882,6 +885,14 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
17th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t xml:space="preserve">17/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">18/03/2020</t>
@@ -765,7 +768,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>660</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="35">
@@ -781,7 +784,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>25</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37">
@@ -789,7 +792,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
@@ -797,7 +800,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39">
@@ -805,7 +808,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40">
@@ -813,7 +816,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41">
@@ -821,7 +824,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
@@ -829,7 +832,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
@@ -837,7 +840,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44">
@@ -845,7 +848,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45">
@@ -853,7 +856,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>153</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46">
@@ -861,7 +864,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47">
@@ -869,7 +872,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48">
@@ -877,7 +880,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49">
@@ -885,7 +888,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -893,6 +896,14 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
18th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">18/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">19/03/2020</t>
@@ -784,7 +787,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>797</v>
+        <v>920</v>
       </c>
     </row>
     <row r="37">
@@ -800,7 +803,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>27</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39">
@@ -808,7 +811,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40">
@@ -816,7 +819,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41">
@@ -824,7 +827,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42">
@@ -832,7 +835,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43">
@@ -840,7 +843,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
@@ -848,7 +851,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45">
@@ -856,7 +859,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46">
@@ -864,7 +867,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>153</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47">
@@ -872,7 +875,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48">
@@ -880,7 +883,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49">
@@ -888,7 +891,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50">
@@ -896,7 +899,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -904,6 +907,14 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -134,7 +134,13 @@
     <t xml:space="preserve">19/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">19/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">20/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">21/03/2020</t>
@@ -739,7 +745,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="31">
@@ -755,7 +761,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>882</v>
+        <v>886</v>
       </c>
     </row>
     <row r="33">
@@ -771,7 +777,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="35">
@@ -787,7 +793,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>920</v>
+        <v>922</v>
       </c>
     </row>
     <row r="37">
@@ -819,7 +825,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>58</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="41">
@@ -827,7 +833,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
@@ -835,7 +841,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43">
@@ -843,7 +849,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44">
@@ -851,7 +857,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45">
@@ -859,7 +865,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46">
@@ -867,7 +873,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47">
@@ -875,7 +881,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>153</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48">
@@ -883,7 +889,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>136</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49">
@@ -891,7 +897,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50">
@@ -899,7 +905,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51">
@@ -907,7 +913,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>187</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52">
@@ -915,6 +921,22 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
22 April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -146,7 +146,13 @@
     <t xml:space="preserve">21/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">21/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">22/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">23/03/2020</t>
@@ -841,7 +847,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>1235</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="43">
@@ -857,7 +863,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>69</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="45">
@@ -865,7 +871,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46">
@@ -873,7 +879,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47">
@@ -881,7 +887,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48">
@@ -889,7 +895,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49">
@@ -897,7 +903,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>153</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50">
@@ -905,7 +911,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>136</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51">
@@ -913,7 +919,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52">
@@ -921,7 +927,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53">
@@ -929,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>187</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54">
@@ -937,6 +943,22 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
24th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -158,7 +158,13 @@
     <t xml:space="preserve">23/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">23/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">24/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">25/03/2020</t>
@@ -879,7 +885,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>34</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="47">
@@ -895,7 +901,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>74</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="49">
@@ -903,7 +909,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50">
@@ -911,7 +917,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>73</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="51">
@@ -919,7 +925,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>153</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52">
@@ -927,7 +933,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>136</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53">
@@ -935,7 +941,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54">
@@ -943,7 +949,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55">
@@ -951,7 +957,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>187</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56">
@@ -959,6 +965,22 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
25th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">25/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">26/03/2020</t>
@@ -917,7 +920,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>1326</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="51">
@@ -933,7 +936,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>73</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53">
@@ -941,7 +944,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>153</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54">
@@ -949,7 +952,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55">
@@ -957,7 +960,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56">
@@ -965,7 +968,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57">
@@ -973,7 +976,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -981,6 +984,14 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
26th April 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">26/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">27/03/2020</t>
@@ -936,7 +939,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>1953</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="53">
@@ -952,7 +955,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>153</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55">
@@ -960,7 +963,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56">
@@ -968,7 +971,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57">
@@ -976,7 +979,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58">
@@ -984,7 +987,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -992,6 +995,14 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="n">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1st May 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t xml:space="preserve">dateannounced</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t xml:space="preserve">26/04/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/05/2020</t>
   </si>
   <si>
     <t xml:space="preserve">27/04/2020</t>
@@ -1023,7 +1026,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>482</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -1031,7 +1034,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>460</v>
+        <v>482</v>
       </c>
     </row>
     <row r="63">
@@ -1039,7 +1042,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>489</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64">
@@ -1047,7 +1050,15 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>488</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="n">
+        <v>561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st May 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
+++ b/covid19_data/excel/national_timeseries/ncov19india_timeserise.xlsx
@@ -1026,7 +1026,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62">
@@ -1050,7 +1050,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="65">

</xml_diff>